<commit_message>
UI_settings data sheet updated
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Settings.data.xlsx
+++ b/tests/artifact/data/UI-Settings.data.xlsx
@@ -2124,8 +2124,8 @@
   <sheetPr/>
   <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
UI-Settings script updated export, import commented
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Settings.data.xlsx
+++ b/tests/artifact/data/UI-Settings.data.xlsx
@@ -2140,8 +2140,8 @@
   <sheetPr/>
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
UI-Settings commented Upload script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Settings.data.xlsx
+++ b/tests/artifact/data/UI-Settings.data.xlsx
@@ -2140,8 +2140,8 @@
   <sheetPr/>
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>

</xml_diff>